<commit_message>
Made an assembler for my assembly language that uses an ISA JSON file. Fixed some stuff in logisim.
</commit_message>
<xml_diff>
--- a/ControlBits.xlsx
+++ b/ControlBits.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geltb\Documents\Documents\8BitCompCamp\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geltb\Documents\Documents\8BitComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FACF4C3-FFD0-4DB0-BCE6-1455AD4523D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E2F2B2-573A-4A8A-ACCE-D7B5B2CF0C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{020BF409-639F-427F-A3D3-84AB3E6F3324}"/>
+    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{020BF409-639F-427F-A3D3-84AB3E6F3324}"/>
   </bookViews>
   <sheets>
     <sheet name="ALU Invert Logic" sheetId="1" r:id="rId1"/>
-    <sheet name="Microcode" sheetId="2" r:id="rId2"/>
-    <sheet name="Opcodes" sheetId="3" r:id="rId3"/>
+    <sheet name="RAMFlags" sheetId="4" r:id="rId2"/>
+    <sheet name="Microcode" sheetId="2" r:id="rId3"/>
+    <sheet name="Opcodes" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="205">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="221">
   <si>
     <t>invert in</t>
   </si>
@@ -652,6 +653,54 @@
   </si>
   <si>
     <t>decr_3</t>
+  </si>
+  <si>
+    <t>R/W = clock nand (not nInput)</t>
+  </si>
+  <si>
+    <t>OD = clock or nOutput</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>write</t>
+  </si>
+  <si>
+    <t>too late to read</t>
+  </si>
+  <si>
+    <t>read/none</t>
+  </si>
+  <si>
+    <t>undefined</t>
+  </si>
+  <si>
+    <t>don't want to write because address is changing</t>
+  </si>
+  <si>
+    <t>read</t>
+  </si>
+  <si>
+    <t>happens potentially on ROM switching</t>
+  </si>
+  <si>
+    <t>R/W</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>mode</t>
+  </si>
+  <si>
+    <t>nInput</t>
+  </si>
+  <si>
+    <t>nOutput</t>
+  </si>
+  <si>
+    <t>clock</t>
   </si>
 </sst>
 </file>
@@ -1042,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48D22FC-E9EE-4EB3-9BDD-D72FBA55914B}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="F47" sqref="F47:J47"/>
     </sheetView>
   </sheetViews>
@@ -2106,6 +2155,214 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F325B02D-82D2-4948-9169-E46195F997C2}">
+  <dimension ref="A1:G14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" t="s">
+        <v>218</v>
+      </c>
+      <c r="D1" t="s">
+        <v>217</v>
+      </c>
+      <c r="E1" t="s">
+        <v>216</v>
+      </c>
+      <c r="F1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>0</v>
+      </c>
+      <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2" t="s">
+        <v>211</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3">
+        <v>1</v>
+      </c>
+      <c r="D3" t="s">
+        <v>213</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" t="s">
+        <v>207</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="F4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" t="s">
+        <v>207</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="F5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7" t="s">
+        <v>210</v>
+      </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
+      <c r="F7">
+        <v>1</v>
+      </c>
+      <c r="G7" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>1</v>
+      </c>
+      <c r="C8">
+        <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>208</v>
+      </c>
+      <c r="E8" t="s">
+        <v>6</v>
+      </c>
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>1</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9" t="s">
+        <v>207</v>
+      </c>
+      <c r="E9">
+        <v>1</v>
+      </c>
+      <c r="F9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>205</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6A8B3EB0-8C8F-4EAD-9366-985685960D26}">
   <dimension ref="A1:U8"/>
   <sheetViews>
@@ -2556,7 +2813,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5679A951-ACB6-4EAB-93C0-EA1B9BA0722E}">
   <dimension ref="A1:N44"/>
   <sheetViews>

</xml_diff>

<commit_message>
Added microcode generation to the assembler
</commit_message>
<xml_diff>
--- a/ControlBits.xlsx
+++ b/ControlBits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geltb\Documents\Documents\8BitComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6E2F2B2-573A-4A8A-ACCE-D7B5B2CF0C3B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C800B021-1D8A-4ED9-A707-5C09CEE53DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{020BF409-639F-427F-A3D3-84AB3E6F3324}"/>
+    <workbookView xWindow="4185" yWindow="4035" windowWidth="21600" windowHeight="11295" xr2:uid="{020BF409-639F-427F-A3D3-84AB3E6F3324}"/>
   </bookViews>
   <sheets>
     <sheet name="ALU Invert Logic" sheetId="1" r:id="rId1"/>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48D22FC-E9EE-4EB3-9BDD-D72FBA55914B}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F47" sqref="F47:J47"/>
+    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2158,8 +2158,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F325B02D-82D2-4948-9169-E46195F997C2}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2367,7 +2367,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2818,7 +2818,7 @@
   <dimension ref="A1:N44"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="N4" sqref="N4"/>
+      <selection activeCell="E5" sqref="A3:E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixed some bugs with the ISA not matching the physical computer
</commit_message>
<xml_diff>
--- a/ControlBits.xlsx
+++ b/ControlBits.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geltb\Documents\Documents\8BitComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C800B021-1D8A-4ED9-A707-5C09CEE53DE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEE3BDC-0927-4F7A-997B-16529291C7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4185" yWindow="4035" windowWidth="21600" windowHeight="11295" xr2:uid="{020BF409-639F-427F-A3D3-84AB3E6F3324}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{020BF409-639F-427F-A3D3-84AB3E6F3324}"/>
   </bookViews>
   <sheets>
     <sheet name="ALU Invert Logic" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="221">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="286" uniqueCount="222">
   <si>
     <t>invert in</t>
   </si>
@@ -205,12 +205,6 @@
     <t>!done</t>
   </si>
   <si>
-    <t>Input</t>
-  </si>
-  <si>
-    <t>Output</t>
-  </si>
-  <si>
     <t>Microcount</t>
   </si>
   <si>
@@ -253,9 +247,6 @@
     <t>InRegSelFromData = input is 011x</t>
   </si>
   <si>
-    <t>nSR B</t>
-  </si>
-  <si>
     <t>ddd00sss</t>
   </si>
   <si>
@@ -701,6 +692,18 @@
   </si>
   <si>
     <t>clock</t>
+  </si>
+  <si>
+    <t>Input/Write</t>
+  </si>
+  <si>
+    <t>Output/Read</t>
+  </si>
+  <si>
+    <t>nR4 B</t>
+  </si>
+  <si>
+    <t>a-b-1</t>
   </si>
 </sst>
 </file>
@@ -1091,7 +1094,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48D22FC-E9EE-4EB3-9BDD-D72FBA55914B}">
   <dimension ref="A1:K49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I20" sqref="I20"/>
     </sheetView>
   </sheetViews>
@@ -1454,7 +1457,7 @@
     </row>
     <row r="20" spans="4:11" x14ac:dyDescent="0.25">
       <c r="E20" t="s">
-        <v>6</v>
+        <v>221</v>
       </c>
       <c r="F20">
         <v>0</v>
@@ -2166,22 +2169,22 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="B1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
       <c r="C1" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="D1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="E1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F1" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -2195,16 +2198,16 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
+        <v>208</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
         <v>211</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -2218,7 +2221,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -2238,7 +2241,7 @@
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E4">
         <v>1</v>
@@ -2247,7 +2250,7 @@
         <v>1</v>
       </c>
       <c r="G4" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2261,7 +2264,7 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E5">
         <v>1</v>
@@ -2281,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="D6" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -2295,7 +2298,7 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="E7" t="s">
         <v>6</v>
@@ -2304,7 +2307,7 @@
         <v>1</v>
       </c>
       <c r="G7" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
@@ -2318,7 +2321,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="E8" t="s">
         <v>6</v>
@@ -2338,7 +2341,7 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -2349,12 +2352,12 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E13" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E14" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
   </sheetData>
@@ -2367,7 +2370,7 @@
   <dimension ref="A1:U8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="N3" sqref="N3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2383,16 +2386,16 @@
   <sheetData>
     <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E1" s="7"/>
       <c r="F1" s="7"/>
@@ -2402,7 +2405,7 @@
       <c r="J1" s="7"/>
       <c r="K1" s="7"/>
       <c r="L1" s="7" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="M1" s="7"/>
       <c r="N1" s="7"/>
@@ -2414,13 +2417,13 @@
     </row>
     <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="D2" s="6" t="s">
-        <v>55</v>
+        <v>218</v>
       </c>
       <c r="E2" s="6"/>
       <c r="F2" s="6"/>
       <c r="G2" s="6"/>
       <c r="H2" s="6" t="s">
-        <v>56</v>
+        <v>219</v>
       </c>
       <c r="I2" s="6"/>
       <c r="J2" s="6"/>
@@ -2429,29 +2432,29 @@
         <v>54</v>
       </c>
       <c r="M2" s="3" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
       <c r="N2" s="3" t="s">
-        <v>71</v>
+        <v>220</v>
       </c>
       <c r="O2" s="6" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="P2" s="6"/>
       <c r="Q2" s="6"/>
       <c r="R2" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="S2" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C3" s="4">
         <v>0</v>
@@ -2505,15 +2508,15 @@
         <v>0</v>
       </c>
       <c r="U3" s="5" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="C4" s="4">
         <v>0</v>
@@ -2567,15 +2570,15 @@
         <v>0</v>
       </c>
       <c r="U4" s="5" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="C5" s="4">
         <v>0</v>
@@ -2631,10 +2634,10 @@
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="C6" s="4">
         <v>0</v>
@@ -2690,10 +2693,10 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>191</v>
+        <v>188</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>192</v>
+        <v>189</v>
       </c>
       <c r="C7" s="4">
         <v>0</v>
@@ -2836,488 +2839,488 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="B1" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="C1" s="4"/>
       <c r="D1" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E1" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="G1" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="K1" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="M1" s="4" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="C2" s="4"/>
       <c r="D2" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="E2" s="4" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="K2" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C3" s="4"/>
       <c r="D3" s="4" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="J3" s="4" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="K3" s="4" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="N3" s="4" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C4" s="4"/>
       <c r="D4" s="4" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="E4" s="4" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="H4" s="4" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="K4" s="4" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>174</v>
+        <v>171</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E5" s="4" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>119</v>
+        <v>116</v>
       </c>
       <c r="H5" s="4" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
       <c r="K5" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
       <c r="N5" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>33</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="E6" s="4" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>120</v>
+        <v>117</v>
       </c>
       <c r="H6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="K6" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="N6" s="4"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>34</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="E7" s="4" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>121</v>
+        <v>118</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J7" s="4" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="K7" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="N7" s="4"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="4" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>32</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="E8" s="4" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>122</v>
+        <v>119</v>
       </c>
       <c r="J8" s="4" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="K8" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="N8" s="4"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>35</v>
       </c>
       <c r="C9" s="4"/>
       <c r="D9" s="4" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="E9" s="4" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>123</v>
+        <v>120</v>
       </c>
       <c r="J9" s="4" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="K9" s="4" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="M9" s="4" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="N9" s="4"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>47</v>
       </c>
       <c r="C10" s="4"/>
       <c r="D10" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="J10" s="4" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
       <c r="K10" s="4" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>48</v>
       </c>
       <c r="C11" s="4"/>
       <c r="D11" s="4" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="H11" s="4" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="K11" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="N11" s="4"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C12" s="4"/>
       <c r="D12" s="4" t="s">
-        <v>126</v>
+        <v>123</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="K12" s="4" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="N12" s="4"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C13" s="4"/>
       <c r="D13" s="4" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="J13" s="4" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="K13" s="4" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="N13" s="4"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="C14" s="4"/>
       <c r="D14" s="4" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="J14" s="4" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="K14" s="4" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="N14" s="4"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C15" s="4"/>
       <c r="D15" s="4" t="s">
-        <v>129</v>
+        <v>126</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="J15" s="4" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>196</v>
+        <v>193</v>
       </c>
       <c r="M15" s="4" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B16" s="4"/>
       <c r="C16" s="4"/>
       <c r="D16" s="4" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="G16" s="4" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="J16" s="4" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="K16" s="4" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="M16" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
     </row>
     <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>46</v>
       </c>
       <c r="C17" s="4"/>
       <c r="D17" s="4" t="s">
-        <v>131</v>
+        <v>128</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="J17" s="4" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="M17" s="4" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
     </row>
     <row r="18" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
DFS works. Assembler now outputs the code stripped of comments and extra newlines to line numbers accurate of PC.
</commit_message>
<xml_diff>
--- a/ControlBits.xlsx
+++ b/ControlBits.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\geltb\Documents\Documents\8BitComputer\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCEE3BDC-0927-4F7A-997B-16529291C7BC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52039352-BE20-4DA7-A0EE-DA80799737A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{020BF409-639F-427F-A3D3-84AB3E6F3324}"/>
   </bookViews>
@@ -1092,20 +1092,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F48D22FC-E9EE-4EB3-9BDD-D72FBA55914B}">
-  <dimension ref="A1:K49"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I20" sqref="I20"/>
+      <selection activeCell="J24" sqref="J24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="H1" t="s">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
@@ -1121,20 +1121,20 @@
       <c r="E2" t="s">
         <v>4</v>
       </c>
-      <c r="H2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="F2" t="s">
         <v>4</v>
       </c>
-      <c r="J2" t="s">
+      <c r="G2" t="s">
         <v>14</v>
       </c>
       <c r="K2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -1150,23 +1150,23 @@
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3" t="s">
-        <v>9</v>
-      </c>
-      <c r="H3">
-        <v>0</v>
-      </c>
-      <c r="I3">
-        <v>0</v>
-      </c>
-      <c r="J3" t="s">
+      <c r="F3">
+        <v>0</v>
+      </c>
+      <c r="G3" t="s">
         <v>16</v>
       </c>
       <c r="K3" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N3" t="s">
+        <v>9</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>0</v>
       </c>
@@ -1182,23 +1182,23 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4" t="s">
-        <v>12</v>
-      </c>
-      <c r="H4">
-        <v>0</v>
-      </c>
-      <c r="I4">
-        <v>0</v>
-      </c>
-      <c r="J4" t="s">
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4" t="s">
         <v>13</v>
       </c>
       <c r="K4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N4" t="s">
+        <v>12</v>
+      </c>
+      <c r="P4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>0</v>
       </c>
@@ -1214,23 +1214,23 @@
       <c r="E5">
         <v>1</v>
       </c>
-      <c r="F5" t="s">
-        <v>10</v>
-      </c>
-      <c r="H5">
-        <v>1</v>
-      </c>
-      <c r="I5">
-        <v>1</v>
-      </c>
-      <c r="J5" t="s">
+      <c r="F5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
         <v>17</v>
       </c>
       <c r="K5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N5" t="s">
+        <v>10</v>
+      </c>
+      <c r="P5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>0</v>
       </c>
@@ -1246,23 +1246,23 @@
       <c r="E6">
         <v>1</v>
       </c>
-      <c r="F6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6">
-        <v>1</v>
-      </c>
-      <c r="I6">
-        <v>1</v>
-      </c>
-      <c r="J6" t="s">
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
         <v>15</v>
       </c>
       <c r="K6" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N6" t="s">
+        <v>11</v>
+      </c>
+      <c r="P6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1278,23 +1278,23 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7">
-        <v>0</v>
-      </c>
-      <c r="I7">
-        <v>0</v>
-      </c>
-      <c r="J7" t="b">
+      <c r="F7">
+        <v>0</v>
+      </c>
+      <c r="G7" t="b">
         <v>1</v>
       </c>
       <c r="K7" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N7" t="s">
+        <v>5</v>
+      </c>
+      <c r="P7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1310,23 +1310,23 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8" t="s">
-        <v>7</v>
-      </c>
-      <c r="H8">
-        <v>0</v>
-      </c>
-      <c r="I8">
-        <v>0</v>
-      </c>
-      <c r="J8" t="b">
+      <c r="F8">
+        <v>0</v>
+      </c>
+      <c r="G8" t="b">
         <v>0</v>
       </c>
       <c r="K8" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N8" t="s">
+        <v>7</v>
+      </c>
+      <c r="P8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1342,17 +1342,17 @@
       <c r="E9" t="s">
         <v>6</v>
       </c>
-      <c r="H9">
-        <v>0</v>
-      </c>
-      <c r="I9">
+      <c r="F9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="P9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1368,38 +1368,38 @@
       <c r="E10">
         <v>1</v>
       </c>
-      <c r="F10" t="s">
-        <v>8</v>
-      </c>
-      <c r="H10">
-        <v>0</v>
-      </c>
-      <c r="I10">
+      <c r="F10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="N10" t="s">
+        <v>8</v>
+      </c>
+      <c r="P10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="F16" t="s">
+        <v>26</v>
+      </c>
+      <c r="G16" t="s">
+        <v>30</v>
+      </c>
+      <c r="H16" t="s">
         <v>25</v>
       </c>
-      <c r="I16" t="s">
-        <v>26</v>
-      </c>
-      <c r="J16" t="s">
-        <v>30</v>
-      </c>
     </row>
     <row r="17" spans="4:11" x14ac:dyDescent="0.25">
-      <c r="F17">
+      <c r="H17">
         <v>2</v>
       </c>
-      <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17">
+      <c r="I17">
+        <v>1</v>
+      </c>
+      <c r="J17">
         <v>0</v>
       </c>
       <c r="K17" t="s">
@@ -1440,7 +1440,7 @@
         <v>0</v>
       </c>
       <c r="G19">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H19">
         <v>0</v>
@@ -1449,7 +1449,7 @@
         <v>0</v>
       </c>
       <c r="J19">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K19" t="s">
         <v>6</v>
@@ -1460,7 +1460,7 @@
         <v>221</v>
       </c>
       <c r="F20">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G20">
         <v>0</v>
@@ -1469,7 +1469,7 @@
         <v>0</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J20">
         <v>0</v>
@@ -1483,19 +1483,19 @@
         <v>8</v>
       </c>
       <c r="F21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G21">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H21">
         <v>0</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J21">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K21" t="s">
         <v>6</v>
@@ -1515,13 +1515,13 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I22">
         <v>0</v>
       </c>
       <c r="J22">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K22">
         <v>0</v>
@@ -1535,10 +1535,10 @@
         <v>0</v>
       </c>
       <c r="G23">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H23">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I23">
         <v>0</v>
@@ -1555,19 +1555,19 @@
         <v>40</v>
       </c>
       <c r="F24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G24">
         <v>0</v>
       </c>
       <c r="H24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J24">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K24">
         <v>1</v>
@@ -1578,16 +1578,16 @@
         <v>41</v>
       </c>
       <c r="F25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G25">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J25">
         <v>1</v>
@@ -1607,13 +1607,13 @@
         <v>0</v>
       </c>
       <c r="G26">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H26">
         <v>0</v>
       </c>
       <c r="I26">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J26">
         <v>0</v>
@@ -1636,10 +1636,10 @@
         <v>0</v>
       </c>
       <c r="I27">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J27">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K27">
         <v>0</v>
@@ -1650,10 +1650,10 @@
         <v>39</v>
       </c>
       <c r="F28">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H28">
         <v>0</v>
@@ -1673,7 +1673,7 @@
         <v>49</v>
       </c>
       <c r="F29">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G29">
         <v>1</v>
@@ -1685,7 +1685,7 @@
         <v>1</v>
       </c>
       <c r="J29">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K29">
         <v>1</v>
@@ -1702,16 +1702,16 @@
         <v>0</v>
       </c>
       <c r="G30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H30">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J30">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K30">
         <v>0</v>
@@ -1728,10 +1728,10 @@
         <v>1</v>
       </c>
       <c r="H31">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I31">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J31">
         <v>1</v>
@@ -1745,19 +1745,19 @@
         <v>34</v>
       </c>
       <c r="F32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H32">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I32">
         <v>1</v>
       </c>
       <c r="J32">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K32">
         <v>1</v>
@@ -1768,13 +1768,13 @@
         <v>35</v>
       </c>
       <c r="F33">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G33">
         <v>1</v>
       </c>
       <c r="H33">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -1794,13 +1794,13 @@
         <v>50</v>
       </c>
       <c r="F34">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G34">
         <v>0</v>
       </c>
       <c r="H34">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I34">
         <v>0</v>
@@ -1817,19 +1817,19 @@
         <v>51</v>
       </c>
       <c r="F35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H35">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I35">
         <v>0</v>
       </c>
       <c r="J35">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K35">
         <v>0</v>
@@ -1846,10 +1846,10 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J36">
         <v>0</v>
@@ -1866,16 +1866,16 @@
         <v>1</v>
       </c>
       <c r="G37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H37">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J37">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K37">
         <v>0</v>
@@ -1883,7 +1883,7 @@
     </row>
     <row r="38" spans="4:11" x14ac:dyDescent="0.25">
       <c r="F38">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G38">
         <v>0</v>
@@ -1895,7 +1895,7 @@
         <v>0</v>
       </c>
       <c r="J38">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K38" t="s">
         <v>6</v>
@@ -1903,10 +1903,10 @@
     </row>
     <row r="39" spans="4:11" x14ac:dyDescent="0.25">
       <c r="F39">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G39">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H39">
         <v>1</v>
@@ -1932,10 +1932,10 @@
         <v>1</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J40">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K40" t="s">
         <v>6</v>
@@ -1946,13 +1946,13 @@
         <v>1</v>
       </c>
       <c r="G41">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H41">
         <v>1</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J41">
         <v>1</v>
@@ -1969,16 +1969,16 @@
         <v>43</v>
       </c>
       <c r="F42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G42">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I42">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J42">
         <v>0</v>
@@ -1992,19 +1992,19 @@
         <v>44</v>
       </c>
       <c r="F43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G43">
         <v>1</v>
       </c>
       <c r="H43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I43">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J43">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K43" t="s">
         <v>6</v>
@@ -2018,10 +2018,10 @@
         <v>1</v>
       </c>
       <c r="G44">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H44">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I44">
         <v>1</v>
@@ -2044,13 +2044,13 @@
         <v>1</v>
       </c>
       <c r="H45">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="I45">
         <v>1</v>
       </c>
       <c r="J45">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K45" t="s">
         <v>6</v>
@@ -2064,19 +2064,19 @@
         <v>47</v>
       </c>
       <c r="F46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G46">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H46">
         <v>1</v>
       </c>
       <c r="I46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J46">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K46">
         <v>0</v>
@@ -2087,7 +2087,7 @@
         <v>48</v>
       </c>
       <c r="F47">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G47">
         <v>1</v>
@@ -2096,7 +2096,7 @@
         <v>1</v>
       </c>
       <c r="I47">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="J47">
         <v>1</v>
@@ -2113,7 +2113,7 @@
         <v>1</v>
       </c>
       <c r="G48">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H48">
         <v>1</v>
@@ -2122,7 +2122,7 @@
         <v>1</v>
       </c>
       <c r="J48">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K48">
         <v>0</v>

</xml_diff>